<commit_message>
Tudo Sprint3 mais documento na sprint4
</commit_message>
<xml_diff>
--- a/Sprint 3/Roteiro_Testes_GestãoSimples.xlsx
+++ b/Sprint 3/Roteiro_Testes_GestãoSimples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julio\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julio\source\repos\GestaoSimples\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356B288F-D440-43DA-9B0E-44B07A78E7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503B2BC2-7004-4AAA-AFD5-B23C8A96CF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="769" firstSheet="14" activeTab="20" xr2:uid="{85B78278-B134-4B28-99AF-1EAE2CD24737}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="769" firstSheet="15" activeTab="22" xr2:uid="{85B78278-B134-4B28-99AF-1EAE2CD24737}"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="280">
   <si>
     <t>Caso de teste</t>
   </si>
@@ -472,9 +472,6 @@
     <t>O sistema aplica as modificações no perfil do usuário.</t>
   </si>
   <si>
-    <t>O sistema redireciona a visão para página de usuário.</t>
-  </si>
-  <si>
     <t>Na tela menu, clicar na opção Fornecedores.</t>
   </si>
   <si>
@@ -646,9 +643,6 @@
     <t>O sistema redireciona a visão para a lista de produtos.</t>
   </si>
   <si>
-    <t>O sistema redireciona a visão para página de produto.</t>
-  </si>
-  <si>
     <t>O sistema aplica as modificações no perfil do produto.</t>
   </si>
   <si>
@@ -839,9 +833,6 @@
   </si>
   <si>
     <t>Tela não implementada na sprint3</t>
-  </si>
-  <si>
-    <t>Ao clicar na linha escolhida, a tela do sistema é redirecionada.</t>
   </si>
   <si>
     <t>Caso de Testes - Visualizar Clientes</t>
@@ -1010,6 +1001,51 @@
   </si>
   <si>
     <t>A guia de compras é apresentada ao usuário com a nova compra incluida na última linha</t>
+  </si>
+  <si>
+    <t>O sistema redireciona a visão para página de edição de usuário.</t>
+  </si>
+  <si>
+    <t>Ao clicar na guia escolhida, a tela do sistema é redirecionada para a guia de produtos.</t>
+  </si>
+  <si>
+    <t>O sistema redireciona a visão para página de alteração de produto.</t>
+  </si>
+  <si>
+    <t>Ao clicar na guia escolhida, a tela do sistema é redirecionada para a guia de Vendas.</t>
+  </si>
+  <si>
+    <t>O sistema apresenta a guia Vendas.</t>
+  </si>
+  <si>
+    <t>O sistema apresenta a guia ProdutosVenda.</t>
+  </si>
+  <si>
+    <t>Ao clicar na guia escolhida, a tela do sistema é redirecionada para Vendas.</t>
+  </si>
+  <si>
+    <t>Ao clicar na linha escolhida, a tela do sistema é redirecionada para a guia ProdutosVenda.</t>
+  </si>
+  <si>
+    <t>Ao clicar na guia escolhida, a tela do sistema é redirecionada para Clientes.</t>
+  </si>
+  <si>
+    <t>O sistema apresenta a guia Clientes.</t>
+  </si>
+  <si>
+    <t>Ao clicar na guia escolhida, a tela do sistema é redirecionada para Compras.</t>
+  </si>
+  <si>
+    <t>O sistema apresenta a guia Compras.</t>
+  </si>
+  <si>
+    <t>Ao clicar na guia escolhida, a tela do sistema é redirecionada para guia de Compras.</t>
+  </si>
+  <si>
+    <t>Ao clicar na linha escolhida, a tela do sistema é redirecionada para a guia ProdutosCompra.</t>
+  </si>
+  <si>
+    <t>O sistema apresenta a guia ProdutosCompra.</t>
   </si>
 </sst>
 </file>
@@ -1372,11 +1408,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1421,22 +1457,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1454,13 +1481,22 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1969,7 +2005,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -1980,7 +2016,7 @@
     </row>
     <row r="2" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="67" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
@@ -1990,12 +2026,12 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
@@ -2004,13 +2040,13 @@
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -2025,9 +2061,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -2037,7 +2073,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26"/>
@@ -2054,7 +2090,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
@@ -2075,7 +2111,7 @@
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25" t="s">
@@ -2088,7 +2124,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26"/>
@@ -2103,10 +2139,10 @@
         <v>32</v>
       </c>
       <c r="B10" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>129</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>130</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="25"/>
@@ -2126,7 +2162,7 @@
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25" t="s">
@@ -2145,7 +2181,7 @@
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25" t="s">
@@ -2158,11 +2194,11 @@
         <v>103</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25" t="s">
@@ -2171,15 +2207,15 @@
       <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="53"/>
     </row>
     <row r="15" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:7" s="16" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2265,7 +2301,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -2286,12 +2322,12 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
@@ -2300,13 +2336,13 @@
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -2321,9 +2357,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -2333,11 +2369,11 @@
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26" t="s">
-        <v>112</v>
+        <v>266</v>
       </c>
       <c r="E6" s="28">
         <v>45573</v>
@@ -2352,11 +2388,11 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -2365,15 +2401,15 @@
       <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:7" s="16" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2423,77 +2459,21 @@
     <row r="30" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="31" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="32" s="14" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-    </row>
-    <row r="34" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-    </row>
-    <row r="36" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-    </row>
-    <row r="41" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-    </row>
-    <row r="43" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-    </row>
-    <row r="45" spans="1:7" s="16" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-    </row>
-    <row r="47" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="14" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="16" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A8:G8"/>
@@ -2536,7 +2516,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -2557,27 +2537,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -2592,14 +2572,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
     </row>
-    <row r="6" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>28</v>
       </c>
@@ -2623,11 +2603,11 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -2640,10 +2620,10 @@
         <v>30</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>57</v>
@@ -2656,7 +2636,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>31</v>
       </c>
@@ -2678,11 +2658,11 @@
         <v>32</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25" t="s">
@@ -2716,7 +2696,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2730,7 +2710,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -2741,7 +2721,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
@@ -2751,27 +2731,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -2786,9 +2766,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -2798,7 +2778,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26"/>
@@ -2815,7 +2795,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
@@ -2836,7 +2816,7 @@
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="26" t="s">
-        <v>153</v>
+        <v>267</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25" t="s">
@@ -2849,7 +2829,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26"/>
@@ -2864,10 +2844,10 @@
         <v>32</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="25"/>
@@ -2887,7 +2867,7 @@
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25" t="s">
@@ -2906,7 +2886,7 @@
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25" t="s">
@@ -2919,11 +2899,11 @@
         <v>103</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25" t="s">
@@ -2932,15 +2912,15 @@
       <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2969,7 +2949,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2983,7 +2963,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -3004,27 +2984,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -3039,9 +3019,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -3051,11 +3031,11 @@
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26" t="s">
-        <v>112</v>
+        <v>268</v>
       </c>
       <c r="E6" s="28">
         <v>45573</v>
@@ -3065,16 +3045,16 @@
       </c>
       <c r="G6" s="25"/>
     </row>
-    <row r="7" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>113</v>
+        <v>269</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -3083,15 +3063,15 @@
       <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3119,8 +3099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA441FA-7B68-4242-A01D-611C4005CEC4}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection sqref="A1:XFD20"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3134,7 +3114,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -3155,27 +3135,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>163</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -3190,14 +3170,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
     </row>
-    <row r="6" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>28</v>
       </c>
@@ -3221,11 +3201,11 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -3238,11 +3218,11 @@
         <v>30</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="26" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25" t="s">
@@ -3255,13 +3235,13 @@
         <v>31</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25" t="s">
@@ -3276,11 +3256,11 @@
         <v>32</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25" t="s">
@@ -3295,11 +3275,11 @@
         <v>99</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25" t="s">
@@ -3312,11 +3292,11 @@
         <v>101</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25" t="s">
@@ -3329,11 +3309,11 @@
         <v>103</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25" t="s">
@@ -3343,14 +3323,14 @@
     </row>
     <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="26" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25" t="s">
@@ -3360,14 +3340,14 @@
     </row>
     <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="26" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="25" t="s">
@@ -3377,14 +3357,14 @@
     </row>
     <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E16" s="25"/>
       <c r="F16" s="25" t="s">
@@ -3394,14 +3374,14 @@
     </row>
     <row r="17" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="25" t="s">
@@ -3411,14 +3391,14 @@
     </row>
     <row r="18" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="25" t="s">
@@ -3428,14 +3408,14 @@
     </row>
     <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="25" t="s">
@@ -3445,14 +3425,14 @@
     </row>
     <row r="20" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E20" s="25"/>
       <c r="F20" s="25" t="s">
@@ -3461,58 +3441,58 @@
       <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:7" s="14" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="57" t="s">
-        <v>199</v>
-      </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="59"/>
+      <c r="A21" s="54" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
     </row>
     <row r="22" spans="1:7" s="14" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="60" t="s">
+      <c r="A22" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="60" t="s">
+      <c r="G22" s="57" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="14" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="61"/>
-      <c r="B23" s="61"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="22"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
     </row>
     <row r="24" spans="1:7" s="16" customFormat="1" ht="59.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E24" s="28">
         <v>45573</v>
@@ -3527,11 +3507,11 @@
         <v>29</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="25" t="s">
@@ -3544,11 +3524,11 @@
         <v>30</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="25" t="s">
@@ -3561,11 +3541,11 @@
         <v>31</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="25" t="s">
@@ -3578,11 +3558,11 @@
         <v>32</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="25" t="s">
@@ -3591,58 +3571,58 @@
       <c r="G28" s="25"/>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="57" t="s">
-        <v>205</v>
-      </c>
-      <c r="B29" s="58"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="59"/>
+      <c r="A29" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="56"/>
     </row>
     <row r="30" spans="1:7" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="60" t="s">
+      <c r="E30" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="60" t="s">
+      <c r="F30" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="60" t="s">
+      <c r="G30" s="57" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="14" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="61"/>
-      <c r="B31" s="61"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="58"/>
       <c r="C31" s="22"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
     </row>
     <row r="32" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E32" s="25"/>
       <c r="F32" s="25" t="s">
@@ -3655,11 +3635,11 @@
         <v>29</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E33" s="25"/>
       <c r="F33" s="25" t="s">
@@ -3672,11 +3652,11 @@
         <v>30</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E34" s="25"/>
       <c r="F34" s="25" t="s">
@@ -3689,11 +3669,11 @@
         <v>31</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E35" s="25"/>
       <c r="F35" s="25" t="s">
@@ -3702,33 +3682,18 @@
       <c r="G35" s="25"/>
     </row>
     <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="62" t="s">
+      <c r="A36" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="64"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
@@ -3738,6 +3703,21 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F20 F24:F28 F32:F35" xr:uid="{2DB5A9F5-6A17-4BAB-849D-00FB985073D1}">
@@ -3753,7 +3733,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3767,7 +3747,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -3788,27 +3768,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -3823,23 +3803,23 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
     </row>
-    <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26" t="s">
-        <v>112</v>
+        <v>271</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="25"/>
@@ -3850,11 +3830,11 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>113</v>
+        <v>269</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
@@ -3865,16 +3845,16 @@
         <v>30</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="26" t="s">
-        <v>218</v>
+        <v>272</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3882,28 +3862,28 @@
         <v>31</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26" t="s">
-        <v>113</v>
+        <v>270</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="64"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3946,7 +3926,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -3967,27 +3947,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>220</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -4002,9 +3982,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -4014,11 +3994,11 @@
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26" t="s">
-        <v>112</v>
+        <v>273</v>
       </c>
       <c r="E6" s="28">
         <v>45573</v>
@@ -4033,11 +4013,11 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>113</v>
+        <v>274</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -4046,15 +4026,15 @@
       <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4083,7 +4063,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4097,7 +4077,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -4118,27 +4098,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>223</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -4153,14 +4133,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
     </row>
-    <row r="6" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>28</v>
       </c>
@@ -4184,11 +4164,11 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -4201,10 +4181,10 @@
         <v>30</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>57</v>
@@ -4217,7 +4197,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>31</v>
       </c>
@@ -4243,7 +4223,7 @@
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="26" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25" t="s">
@@ -4291,7 +4271,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -4302,7 +4282,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="67" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
@@ -4312,27 +4292,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>231</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -4347,9 +4327,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -4359,7 +4339,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26"/>
@@ -4376,7 +4356,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
@@ -4397,7 +4377,7 @@
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="26" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25" t="s">
@@ -4410,11 +4390,11 @@
         <v>31</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25" t="s">
@@ -4427,13 +4407,13 @@
         <v>32</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>237</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>240</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25" t="s">
@@ -4452,7 +4432,7 @@
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="26" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25" t="s">
@@ -4471,7 +4451,7 @@
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="26" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25" t="s">
@@ -4484,11 +4464,11 @@
         <v>103</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="26" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25" t="s">
@@ -4497,15 +4477,15 @@
       <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4557,17 +4537,17 @@
       <c r="D5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35" t="s">
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="35"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C6" s="10">
@@ -4576,17 +4556,17 @@
       <c r="D6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34" t="s">
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="34"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C7" s="10"/>
@@ -4596,99 +4576,106 @@
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
       <c r="I7" s="38"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C8" s="10"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C9" s="10"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C10" s="10"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C11" s="10"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C12" s="10"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C13" s="10"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C15" s="10"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E10:I10"/>
     <mergeCell ref="E5:I5"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="E12:I12"/>
@@ -4704,13 +4691,6 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E10:I10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
@@ -4732,7 +4712,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4746,7 +4726,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -4767,27 +4747,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>245</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>242</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -4802,9 +4782,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -4814,11 +4794,11 @@
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26" t="s">
-        <v>112</v>
+        <v>275</v>
       </c>
       <c r="E6" s="28">
         <v>45573</v>
@@ -4828,16 +4808,16 @@
       </c>
       <c r="G6" s="25"/>
     </row>
-    <row r="7" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>113</v>
+        <v>276</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -4846,15 +4826,15 @@
       <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4882,7 +4862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F23CDF-3DAC-4D07-8371-6416C43CC738}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -4897,7 +4877,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -4918,27 +4898,27 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>248</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
     </row>
-    <row r="4" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -4953,14 +4933,14 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
     </row>
-    <row r="6" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>28</v>
       </c>
@@ -4984,11 +4964,11 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -5001,11 +4981,11 @@
         <v>99</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="26" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25" t="s">
@@ -5018,11 +4998,11 @@
         <v>101</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25" t="s">
@@ -5035,11 +5015,11 @@
         <v>103</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="26" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25" t="s">
@@ -5049,14 +5029,14 @@
     </row>
     <row r="11" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="26" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25" t="s">
@@ -5066,14 +5046,14 @@
     </row>
     <row r="12" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="26" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="25" t="s">
@@ -5083,14 +5063,14 @@
     </row>
     <row r="13" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25" t="s">
@@ -5100,14 +5080,14 @@
     </row>
     <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="26" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25" t="s">
@@ -5117,14 +5097,14 @@
     </row>
     <row r="15" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="26" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="25" t="s">
@@ -5171,7 +5151,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -5192,12 +5172,12 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>250</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
@@ -5206,13 +5186,13 @@
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -5227,38 +5207,38 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
     </row>
-    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26" t="s">
-        <v>112</v>
+        <v>277</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
     </row>
-    <row r="7" spans="1:7" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
@@ -5269,16 +5249,16 @@
         <v>30</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="26" t="s">
-        <v>218</v>
+        <v>278</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
@@ -5286,28 +5266,28 @@
         <v>31</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="26" t="s">
-        <v>113</v>
+        <v>279</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="64"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -5335,7 +5315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6EC4E5-D49C-4F06-B467-530A2902E467}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -5597,8 +5577,8 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD20"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5614,69 +5594,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="56"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="64"/>
     </row>
     <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="57" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
-      <c r="B5" s="61"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
     </row>
     <row r="6" spans="1:7" s="16" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
@@ -5751,47 +5731,47 @@
       <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="59"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="56"/>
     </row>
     <row r="11" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="60" t="s">
+      <c r="G11" s="57" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
-      <c r="B12" s="61"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="22"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
     </row>
     <row r="13" spans="1:7" s="16" customFormat="1" ht="59.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
@@ -5887,26 +5867,26 @@
       <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="64"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="59"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
     </row>
     <row r="20" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
@@ -5995,6 +5975,15 @@
     <row r="66" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A10:G10"/>
@@ -6004,15 +5993,6 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
@@ -6054,69 +6034,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="53"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="56"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="64"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="57" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
-      <c r="B5" s="61"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
     </row>
     <row r="6" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
@@ -6231,12 +6211,12 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
@@ -6245,13 +6225,13 @@
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -6266,9 +6246,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -6460,8 +6440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7C1EDE-8C35-4A7F-8721-F656F8BF4A6D}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G14"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6499,12 +6479,12 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
@@ -6513,13 +6493,13 @@
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -6534,9 +6514,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -6584,7 +6564,7 @@
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="26" t="s">
-        <v>109</v>
+        <v>265</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="25" t="s">
@@ -6678,15 +6658,15 @@
       <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="53"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
@@ -6805,12 +6785,12 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
@@ -6819,13 +6799,13 @@
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -6840,9 +6820,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -6852,11 +6832,11 @@
         <v>28</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" s="28">
         <v>45573</v>
@@ -6871,11 +6851,11 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -6884,15 +6864,15 @@
       <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6991,7 +6971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9173E3E2-35F9-4274-9586-D1AEF990CB03}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -7009,7 +6989,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -7030,12 +7010,12 @@
       <c r="G2" s="68"/>
     </row>
     <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
+      <c r="A3" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="70"/>
@@ -7044,13 +7024,13 @@
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="71" t="s">
@@ -7065,9 +7045,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="71"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="58"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="72"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
@@ -7096,11 +7076,11 @@
         <v>29</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="25" t="s">
@@ -7113,10 +7093,10 @@
         <v>30</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>57</v>
@@ -7151,11 +7131,11 @@
         <v>32</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25" t="s">
@@ -7168,7 +7148,7 @@
         <v>99</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="26"/>
@@ -7252,6 +7232,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B18A9C64F345EF489DAF5C40B316348D" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="931974aea73882e97edb02920ec76d3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="361f150f-a374-46e3-95a7-056438591200" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="967eb02429ec9ddc08128a799e5775b0" ns2:_="">
     <xsd:import namespace="361f150f-a374-46e3-95a7-056438591200"/>
@@ -7419,16 +7408,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398F9E7A-BFE9-4D97-B975-D036BE08F801}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BFA2B47-5CA0-4619-B871-CA2C9F988427}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7444,12 +7432,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398F9E7A-BFE9-4D97-B975-D036BE08F801}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>